<commit_message>
updated final cut food webs and created CSVs of nodes and interactions for both
</commit_message>
<xml_diff>
--- a/Published_webs/Dryad/Dryad_doi_citations.xlsx
+++ b/Published_webs/Dryad/Dryad_doi_citations.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ana/Dropbox/2020/Dissertation/DNA_predators/Published_webs/Dryad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E54B8A-80B8-8946-B0DE-5BBA655A83E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759DF004-A6B2-2C45-94F8-AE60CCEF3462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="15140" windowHeight="14720" xr2:uid="{5D6EE8B6-8AFD-C447-9F9F-27D6918F0B10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -374,9 +374,6 @@
     <t>Utility?</t>
   </si>
   <si>
-    <t>fw_broom useful, downloaded body sizes from original citation Brose</t>
-  </si>
-  <si>
     <t>no - low resolution and few interactions recorded</t>
   </si>
   <si>
@@ -384,6 +381,9 @@
   </si>
   <si>
     <t>Food web?</t>
+  </si>
+  <si>
+    <t>fw_broom useful, downloaded body sizes from original citation Brose only 56 nodes</t>
   </si>
 </sst>
 </file>
@@ -773,12 +773,13 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -807,7 +808,7 @@
         <v>112</v>
       </c>
       <c r="I1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -910,32 +911,32 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:9" s="7" customFormat="1">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="C6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1080,7 +1081,7 @@
         <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18">
@@ -1106,7 +1107,7 @@
         <v>84</v>
       </c>
       <c r="H13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:9">

</xml_diff>

<commit_message>
added and curated data from Dryad sources
</commit_message>
<xml_diff>
--- a/Published_webs/Dryad/Dryad_doi_citations.xlsx
+++ b/Published_webs/Dryad/Dryad_doi_citations.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ana/Dropbox/2020/Dissertation/DNA_predators/Published_webs/Dryad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759DF004-A6B2-2C45-94F8-AE60CCEF3462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495FCD62-0E9F-514F-9D4C-13F238391041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="15140" windowHeight="14720" xr2:uid="{5D6EE8B6-8AFD-C447-9F9F-27D6918F0B10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="120">
   <si>
     <t>DOI</t>
   </si>
@@ -371,9 +371,6 @@
     <t>Molecular</t>
   </si>
   <si>
-    <t>Utility?</t>
-  </si>
-  <si>
     <t>no - low resolution and few interactions recorded</t>
   </si>
   <si>
@@ -384,13 +381,25 @@
   </si>
   <si>
     <t>fw_broom useful, downloaded body sizes from original citation Brose only 56 nodes</t>
+  </si>
+  <si>
+    <t>Family or lower?</t>
+  </si>
+  <si>
+    <t>maybe</t>
+  </si>
+  <si>
+    <t>is this considered parasitism?</t>
+  </si>
+  <si>
+    <t>this paper is RAD in validating the individual foraging specializatin in invertebrates idea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -414,6 +423,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -446,15 +461,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -770,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4591C1AC-4E4C-0A4F-9F0D-7B35B50A5E01}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -782,7 +798,7 @@
     <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -805,142 +821,157 @@
         <v>111</v>
       </c>
       <c r="H1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18">
+      <c r="A3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18">
+      <c r="A4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="4" customFormat="1">
+      <c r="A6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18">
-      <c r="A3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18">
-      <c r="A4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="18">
-      <c r="A5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="7" customFormat="1">
-      <c r="A6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="G6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -962,11 +993,8 @@
       <c r="G7" t="s">
         <v>84</v>
       </c>
-      <c r="H7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -988,11 +1016,8 @@
       <c r="G8" t="s">
         <v>84</v>
       </c>
-      <c r="H8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="18">
+    </row>
+    <row r="9" spans="1:10" ht="18">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -1011,11 +1036,8 @@
       <c r="G9" t="s">
         <v>84</v>
       </c>
-      <c r="H9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18">
+    </row>
+    <row r="10" spans="1:10" ht="18">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -1034,11 +1056,8 @@
       <c r="G10" t="s">
         <v>84</v>
       </c>
-      <c r="H10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="18">
+    </row>
+    <row r="11" spans="1:10" ht="18">
       <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
@@ -1057,11 +1076,8 @@
       <c r="G11" t="s">
         <v>84</v>
       </c>
-      <c r="H11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1081,10 +1097,10 @@
         <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1107,10 +1123,10 @@
         <v>84</v>
       </c>
       <c r="H13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1136,7 +1152,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -1156,7 +1172,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1682,6 +1698,7 @@
     <hyperlink ref="B27" r:id="rId21" display="https://doi.org/10.5061/dryad.1d8761h1" xr:uid="{93A42647-31FA-974E-9B34-8BBCA01471BE}"/>
     <hyperlink ref="B36" r:id="rId22" display="https://doi.org/10.5061/dryad.95262" xr:uid="{0B03963A-EA48-3C4D-B9DF-B47F68DB0233}"/>
     <hyperlink ref="B37" r:id="rId23" display="https://doi.org/10.5061/dryad.311mm" xr:uid="{7DE8350E-4D97-A140-850D-4CDEA71B4A45}"/>
+    <hyperlink ref="A5" r:id="rId24" xr:uid="{8868889A-57A2-224F-A92C-D3D40B4C2A9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>